<commit_message>
next version of three good bot
</commit_message>
<xml_diff>
--- a/slackbot_config.xlsx
+++ b/slackbot_config.xlsx
@@ -4,21 +4,21 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="OAuth_codes" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="messaging_queue" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -41,12 +41,6 @@
       <family val="0"/>
       <sz val="10"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -66,40 +60,40 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="1"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="5" name="Percent" xfId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -395,19 +389,19 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B4" activeCellId="0" pane="topLeft" sqref="B4"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="8.529999999999999"/>
-    <col customWidth="1" max="2" min="2" style="3" width="25"/>
-    <col customWidth="1" max="3" min="3" style="3" width="34"/>
-    <col customWidth="1" max="1025" min="4" style="3" width="8.529999999999999"/>
+    <col width="10.96" customWidth="1" style="3" min="1" max="1"/>
+    <col width="25" customWidth="1" style="3" min="2" max="2"/>
+    <col width="34" customWidth="1" style="3" min="3" max="3"/>
+    <col width="8.529999999999999" customWidth="1" style="3" min="4" max="1025"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="14.4" r="1" s="4">
+    <row r="1" ht="14.4" customHeight="1" s="4">
       <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Client</t>
@@ -424,7 +418,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="2" s="4">
+    <row r="2" ht="13.8" customHeight="1" s="4">
       <c r="A2" s="3" t="inlineStr">
         <is>
           <t>admin_test</t>
@@ -441,7 +435,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="3" s="4">
+    <row r="3" ht="13.8" customHeight="1" s="4">
       <c r="A3" s="3" t="inlineStr">
         <is>
           <t>customer1</t>
@@ -458,7 +452,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="4" s="4">
+    <row r="4" ht="13.8" customHeight="1" s="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
           <t>admin</t>
@@ -475,7 +469,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="5" s="4">
+    <row r="5" ht="13.8" customHeight="1" s="4">
       <c r="A5" s="3" t="inlineStr">
         <is>
           <t>Three Good</t>
@@ -492,11 +486,11 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="6" s="4"/>
+    <row r="6" ht="13.8" customHeight="1" s="4"/>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
@@ -506,18 +500,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B4" activeCellId="0" pane="topLeft" sqref="B4"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="3" width="8.529999999999999"/>
+    <col width="10.96" customWidth="1" style="3" min="1" max="1"/>
+    <col width="8.529999999999999" customWidth="1" style="3" min="2" max="2"/>
+    <col width="54.34" customWidth="1" style="3" min="3" max="3"/>
+    <col width="8.529999999999999" customWidth="1" style="3" min="4" max="1025"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="14.4" r="1" s="4">
+    <row r="1" ht="14.4" customHeight="1" s="4">
       <c r="A1" s="3" t="inlineStr">
         <is>
           <t>client_to</t>
@@ -544,7 +541,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="2" s="4">
+    <row r="2" ht="13.8" customHeight="1" s="4">
       <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Three Good</t>
@@ -560,11 +557,11 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>2020-03-06 14:47:41</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.8" r="3" s="4">
+          <t>2020-03-27 19:19:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="13.8" customHeight="1" s="4">
       <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Three Good</t>
@@ -580,11 +577,11 @@
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>2020-03-06 14:47:41</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="202.95" r="4" s="4">
+          <t>2020-03-27 19:19:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="202.95" customHeight="1" s="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
           <t>customer1</t>
@@ -606,18 +603,43 @@
 Remember to drink more water to help more people! </t>
         </is>
       </c>
-      <c r="D4" t="b">
+      <c r="D4" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2020-03-06 14:47:41</t>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>2020-03-27 19:19:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="13.8" customHeight="1" s="4">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Three Good</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>dan</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2020-03-27 19:19:50</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
</xml_diff>